<commit_message>
New Product entreprenuerial activity GEM new dataset is updated
</commit_message>
<xml_diff>
--- a/data/[R] [GEM] New product entrepreneurial activity.xlsx
+++ b/data/[R] [GEM] New product entrepreneurial activity.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="14355" windowHeight="6720"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="6465"/>
   </bookViews>
   <sheets>
-    <sheet name="New product entrepreneurial act" sheetId="1" r:id="rId1"/>
+    <sheet name="GEM_Dataset_20140421041552" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="102">
-  <si>
-    <t>All Countries + All Years + TEAYYNWP</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="105">
+  <si>
+    <t>All Countries + Multiple Years + TEAYYNWP</t>
   </si>
   <si>
     <t>New Product early-stage Entrepreneurial Activity</t>
@@ -94,9 +94,6 @@
     <t>Denmark</t>
   </si>
   <si>
-    <t>Diego Garcia</t>
-  </si>
-  <si>
     <t>Dominican Republic</t>
   </si>
   <si>
@@ -181,9 +178,15 @@
     <t>Lebanon</t>
   </si>
   <si>
+    <t>Libya</t>
+  </si>
+  <si>
     <t>Lithuania</t>
   </si>
   <si>
+    <t>Luxembourg</t>
+  </si>
+  <si>
     <t>Macedonia</t>
   </si>
   <si>
@@ -268,6 +271,9 @@
     <t>Spain</t>
   </si>
   <si>
+    <t>Suriname</t>
+  </si>
+  <si>
     <t>Sweden</t>
   </si>
   <si>
@@ -314,6 +320,9 @@
   </si>
   <si>
     <t>Venezuela</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
   </si>
   <si>
     <t>Yemen</t>
@@ -1148,9 +1157,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L102"/>
+  <dimension ref="A1:L105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1174,37 +1185,37 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="C5">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="D5">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="E5">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="F5">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="G5">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="H5">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="I5">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="J5">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="K5">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="L5">
-        <v>2012</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1229,20 +1240,20 @@
       <c r="G6" t="s">
         <v>5</v>
       </c>
-      <c r="H6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6">
+      <c r="H6">
         <v>53</v>
       </c>
-      <c r="J6" t="s">
-        <v>5</v>
+      <c r="I6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>43</v>
       </c>
       <c r="K6">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="L6">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1264,23 +1275,23 @@
       <c r="F7" t="s">
         <v>5</v>
       </c>
-      <c r="G7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7">
+      <c r="G7">
         <v>32</v>
       </c>
-      <c r="I7" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7">
+      <c r="H7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7">
         <v>32</v>
       </c>
-      <c r="K7" t="s">
-        <v>5</v>
+      <c r="J7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>55</v>
       </c>
       <c r="L7">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1314,11 +1325,11 @@
       <c r="J8" t="s">
         <v>5</v>
       </c>
-      <c r="K8" t="s">
-        <v>5</v>
-      </c>
-      <c r="L8">
+      <c r="K8">
         <v>62</v>
+      </c>
+      <c r="L8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1326,37 +1337,37 @@
         <v>8</v>
       </c>
       <c r="B9">
+        <v>42</v>
+      </c>
+      <c r="C9">
+        <v>60</v>
+      </c>
+      <c r="D9">
+        <v>66</v>
+      </c>
+      <c r="E9">
+        <v>71</v>
+      </c>
+      <c r="F9">
+        <v>60</v>
+      </c>
+      <c r="G9">
+        <v>70</v>
+      </c>
+      <c r="H9">
+        <v>77</v>
+      </c>
+      <c r="I9">
+        <v>53</v>
+      </c>
+      <c r="J9">
         <v>47</v>
       </c>
-      <c r="C9">
+      <c r="K9">
         <v>42</v>
       </c>
-      <c r="D9">
-        <v>60</v>
-      </c>
-      <c r="E9">
-        <v>66</v>
-      </c>
-      <c r="F9">
-        <v>71</v>
-      </c>
-      <c r="G9">
-        <v>60</v>
-      </c>
-      <c r="H9">
-        <v>70</v>
-      </c>
-      <c r="I9">
-        <v>77</v>
-      </c>
-      <c r="J9">
-        <v>53</v>
-      </c>
-      <c r="K9">
-        <v>47</v>
-      </c>
       <c r="L9">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1364,34 +1375,34 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C10">
         <v>39</v>
       </c>
       <c r="D10">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E10">
-        <v>32</v>
-      </c>
-      <c r="F10">
         <v>36</v>
       </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10" t="s">
         <v>5</v>
       </c>
-      <c r="I10" t="s">
-        <v>5</v>
+      <c r="I10">
+        <v>36</v>
       </c>
       <c r="J10">
-        <v>36</v>
-      </c>
-      <c r="K10">
         <v>41</v>
+      </c>
+      <c r="K10" t="s">
+        <v>5</v>
       </c>
       <c r="L10" t="s">
         <v>5</v>
@@ -1407,18 +1418,18 @@
       <c r="C11" t="s">
         <v>5</v>
       </c>
-      <c r="D11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11">
+      <c r="D11">
         <v>44</v>
       </c>
-      <c r="F11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G11">
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11">
         <v>44</v>
       </c>
+      <c r="G11" t="s">
+        <v>5</v>
+      </c>
       <c r="H11" t="s">
         <v>5</v>
       </c>
@@ -1428,11 +1439,11 @@
       <c r="J11" t="s">
         <v>5</v>
       </c>
-      <c r="K11" t="s">
-        <v>5</v>
-      </c>
-      <c r="L11">
+      <c r="K11">
         <v>48</v>
+      </c>
+      <c r="L11" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1463,11 +1474,11 @@
       <c r="I12" t="s">
         <v>5</v>
       </c>
-      <c r="J12" t="s">
-        <v>5</v>
-      </c>
-      <c r="K12">
+      <c r="J12">
         <v>11</v>
+      </c>
+      <c r="K12" t="s">
+        <v>5</v>
       </c>
       <c r="L12" t="s">
         <v>5</v>
@@ -1501,8 +1512,8 @@
       <c r="I13" t="s">
         <v>5</v>
       </c>
-      <c r="J13" t="s">
-        <v>5</v>
+      <c r="J13">
+        <v>21</v>
       </c>
       <c r="K13">
         <v>21</v>
@@ -1516,37 +1527,37 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C14">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D14">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E14">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F14">
+        <v>49</v>
+      </c>
+      <c r="G14">
+        <v>43</v>
+      </c>
+      <c r="H14">
+        <v>42</v>
+      </c>
+      <c r="I14">
+        <v>41</v>
+      </c>
+      <c r="J14">
+        <v>34</v>
+      </c>
+      <c r="K14">
+        <v>53</v>
+      </c>
+      <c r="L14">
         <v>38</v>
-      </c>
-      <c r="G14">
-        <v>49</v>
-      </c>
-      <c r="H14">
-        <v>43</v>
-      </c>
-      <c r="I14">
-        <v>42</v>
-      </c>
-      <c r="J14">
-        <v>41</v>
-      </c>
-      <c r="K14">
-        <v>34</v>
-      </c>
-      <c r="L14">
-        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1568,17 +1579,17 @@
       <c r="F15" t="s">
         <v>5</v>
       </c>
-      <c r="G15" t="s">
-        <v>5</v>
-      </c>
-      <c r="H15">
+      <c r="G15">
         <v>36</v>
       </c>
-      <c r="I15" t="s">
-        <v>5</v>
-      </c>
-      <c r="J15">
+      <c r="H15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15">
         <v>36</v>
+      </c>
+      <c r="J15" t="s">
+        <v>5</v>
       </c>
       <c r="K15" t="s">
         <v>5</v>
@@ -1606,23 +1617,23 @@
       <c r="F16" t="s">
         <v>5</v>
       </c>
-      <c r="G16" t="s">
-        <v>5</v>
+      <c r="G16">
+        <v>18</v>
       </c>
       <c r="H16">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="I16">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="J16">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="K16">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L16">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1656,11 +1667,11 @@
       <c r="J17" t="s">
         <v>5</v>
       </c>
-      <c r="K17" t="s">
-        <v>5</v>
+      <c r="K17">
+        <v>34</v>
       </c>
       <c r="L17">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1668,34 +1679,34 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C18">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D18">
         <v>16</v>
       </c>
       <c r="E18">
+        <v>23</v>
+      </c>
+      <c r="F18">
+        <v>21</v>
+      </c>
+      <c r="G18">
         <v>16</v>
       </c>
-      <c r="F18">
-        <v>23</v>
-      </c>
-      <c r="G18">
-        <v>21</v>
-      </c>
       <c r="H18">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I18">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="J18">
-        <v>17</v>
-      </c>
-      <c r="K18">
         <v>11</v>
+      </c>
+      <c r="K18" t="s">
+        <v>5</v>
       </c>
       <c r="L18" t="s">
         <v>5</v>
@@ -1706,20 +1717,20 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C19">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="D19">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E19">
-        <v>50</v>
-      </c>
-      <c r="F19">
         <v>44</v>
       </c>
+      <c r="F19" t="s">
+        <v>5</v>
+      </c>
       <c r="G19" t="s">
         <v>5</v>
       </c>
@@ -1735,8 +1746,8 @@
       <c r="K19" t="s">
         <v>5</v>
       </c>
-      <c r="L19" t="s">
-        <v>5</v>
+      <c r="L19">
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1744,37 +1755,37 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>81</v>
-      </c>
-      <c r="C20">
         <v>88</v>
       </c>
-      <c r="D20" t="s">
-        <v>5</v>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>66</v>
       </c>
       <c r="E20">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="F20">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G20">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="H20">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="I20">
+        <v>85</v>
+      </c>
+      <c r="J20">
         <v>90</v>
       </c>
-      <c r="J20">
+      <c r="K20">
+        <v>88</v>
+      </c>
+      <c r="L20">
         <v>85</v>
-      </c>
-      <c r="K20">
-        <v>90</v>
-      </c>
-      <c r="L20">
-        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1782,34 +1793,34 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>15</v>
-      </c>
-      <c r="C21">
         <v>30</v>
       </c>
-      <c r="D21" t="s">
-        <v>5</v>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>41</v>
       </c>
       <c r="E21">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="F21">
-        <v>52</v>
-      </c>
-      <c r="G21">
         <v>73</v>
       </c>
-      <c r="H21" t="s">
-        <v>5</v>
-      </c>
-      <c r="I21">
+      <c r="G21" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21">
         <v>61</v>
       </c>
-      <c r="J21" t="s">
-        <v>5</v>
-      </c>
-      <c r="K21">
+      <c r="I21" t="s">
+        <v>5</v>
+      </c>
+      <c r="J21">
         <v>60</v>
+      </c>
+      <c r="K21" t="s">
+        <v>5</v>
       </c>
       <c r="L21" t="s">
         <v>5</v>
@@ -1828,29 +1839,29 @@
       <c r="D22" t="s">
         <v>5</v>
       </c>
-      <c r="E22" t="s">
-        <v>5</v>
+      <c r="E22">
+        <v>50</v>
       </c>
       <c r="F22">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G22">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H22">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="I22">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="J22">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="K22">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="L22">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1884,11 +1895,11 @@
       <c r="J23" t="s">
         <v>5</v>
       </c>
-      <c r="K23" t="s">
-        <v>5</v>
-      </c>
-      <c r="L23">
+      <c r="K23">
         <v>27</v>
+      </c>
+      <c r="L23" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1896,34 +1907,34 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C24">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D24">
+        <v>32</v>
+      </c>
+      <c r="E24">
         <v>30</v>
-      </c>
-      <c r="E24">
-        <v>32</v>
       </c>
       <c r="F24">
         <v>30</v>
       </c>
       <c r="G24">
+        <v>22</v>
+      </c>
+      <c r="H24">
+        <v>23</v>
+      </c>
+      <c r="I24">
+        <v>25</v>
+      </c>
+      <c r="J24">
+        <v>38</v>
+      </c>
+      <c r="K24">
         <v>30</v>
-      </c>
-      <c r="H24">
-        <v>22</v>
-      </c>
-      <c r="I24">
-        <v>23</v>
-      </c>
-      <c r="J24">
-        <v>25</v>
-      </c>
-      <c r="K24">
-        <v>38</v>
       </c>
       <c r="L24">
         <v>30</v>
@@ -1942,12 +1953,12 @@
       <c r="D25" t="s">
         <v>5</v>
       </c>
-      <c r="E25" t="s">
-        <v>5</v>
-      </c>
-      <c r="F25">
+      <c r="E25">
         <v>55</v>
       </c>
+      <c r="F25" t="s">
+        <v>5</v>
+      </c>
       <c r="G25" t="s">
         <v>5</v>
       </c>
@@ -1957,14 +1968,14 @@
       <c r="I25" t="s">
         <v>5</v>
       </c>
-      <c r="J25" t="s">
-        <v>5</v>
-      </c>
-      <c r="K25">
+      <c r="J25">
         <v>59</v>
       </c>
-      <c r="L25" t="s">
-        <v>5</v>
+      <c r="K25" t="s">
+        <v>5</v>
+      </c>
+      <c r="L25">
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1972,37 +1983,37 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C26">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D26">
         <v>53</v>
       </c>
       <c r="E26">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F26">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G26">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="H26">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="I26">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="J26">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="K26">
-        <v>67</v>
-      </c>
-      <c r="L26">
         <v>61</v>
+      </c>
+      <c r="L26" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2021,14 +2032,14 @@
       <c r="E27" t="s">
         <v>5</v>
       </c>
-      <c r="F27" t="s">
-        <v>5</v>
-      </c>
-      <c r="G27" t="s">
-        <v>5</v>
-      </c>
-      <c r="H27" t="s">
-        <v>5</v>
+      <c r="F27">
+        <v>31</v>
+      </c>
+      <c r="G27">
+        <v>35</v>
+      </c>
+      <c r="H27">
+        <v>39</v>
       </c>
       <c r="I27" t="s">
         <v>5</v>
@@ -2039,8 +2050,8 @@
       <c r="K27" t="s">
         <v>5</v>
       </c>
-      <c r="L27">
-        <v>21</v>
+      <c r="L27" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -2050,8 +2061,8 @@
       <c r="B28" t="s">
         <v>5</v>
       </c>
-      <c r="C28" t="s">
-        <v>5</v>
+      <c r="C28">
+        <v>76</v>
       </c>
       <c r="D28" t="s">
         <v>5</v>
@@ -2063,22 +2074,22 @@
         <v>5</v>
       </c>
       <c r="G28">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="H28">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="I28">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J28" t="s">
         <v>5</v>
       </c>
-      <c r="K28" t="s">
-        <v>5</v>
-      </c>
-      <c r="L28" t="s">
-        <v>5</v>
+      <c r="K28">
+        <v>65</v>
+      </c>
+      <c r="L28">
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -2091,8 +2102,8 @@
       <c r="C29" t="s">
         <v>5</v>
       </c>
-      <c r="D29">
-        <v>76</v>
+      <c r="D29" t="s">
+        <v>5</v>
       </c>
       <c r="E29" t="s">
         <v>5</v>
@@ -2100,23 +2111,23 @@
       <c r="F29" t="s">
         <v>5</v>
       </c>
-      <c r="G29" t="s">
-        <v>5</v>
-      </c>
-      <c r="H29">
-        <v>45</v>
-      </c>
-      <c r="I29">
-        <v>15</v>
-      </c>
-      <c r="J29">
-        <v>38</v>
-      </c>
-      <c r="K29" t="s">
-        <v>5</v>
-      </c>
-      <c r="L29">
-        <v>65</v>
+      <c r="G29">
+        <v>28</v>
+      </c>
+      <c r="H29" t="s">
+        <v>5</v>
+      </c>
+      <c r="I29" t="s">
+        <v>5</v>
+      </c>
+      <c r="J29" t="s">
+        <v>5</v>
+      </c>
+      <c r="K29">
+        <v>28</v>
+      </c>
+      <c r="L29" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -2141,8 +2152,8 @@
       <c r="G30" t="s">
         <v>5</v>
       </c>
-      <c r="H30">
-        <v>28</v>
+      <c r="H30" t="s">
+        <v>5</v>
       </c>
       <c r="I30" t="s">
         <v>5</v>
@@ -2150,11 +2161,11 @@
       <c r="J30" t="s">
         <v>5</v>
       </c>
-      <c r="K30" t="s">
-        <v>5</v>
-      </c>
-      <c r="L30">
-        <v>28</v>
+      <c r="K30">
+        <v>56</v>
+      </c>
+      <c r="L30" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -2188,11 +2199,11 @@
       <c r="J31" t="s">
         <v>5</v>
       </c>
-      <c r="K31" t="s">
-        <v>5</v>
+      <c r="K31">
+        <v>51</v>
       </c>
       <c r="L31">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -2226,49 +2237,49 @@
       <c r="J32" t="s">
         <v>5</v>
       </c>
-      <c r="K32" t="s">
-        <v>5</v>
-      </c>
-      <c r="L32">
-        <v>51</v>
+      <c r="K32">
+        <v>23</v>
+      </c>
+      <c r="L32" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" t="s">
-        <v>5</v>
-      </c>
-      <c r="F33" t="s">
-        <v>5</v>
-      </c>
-      <c r="G33" t="s">
-        <v>5</v>
-      </c>
-      <c r="H33" t="s">
-        <v>5</v>
-      </c>
-      <c r="I33" t="s">
-        <v>5</v>
-      </c>
-      <c r="J33" t="s">
-        <v>5</v>
-      </c>
-      <c r="K33" t="s">
-        <v>5</v>
+      <c r="B33">
+        <v>40</v>
+      </c>
+      <c r="C33">
+        <v>41</v>
+      </c>
+      <c r="D33">
+        <v>44</v>
+      </c>
+      <c r="E33">
+        <v>52</v>
+      </c>
+      <c r="F33">
+        <v>48</v>
+      </c>
+      <c r="G33">
+        <v>44</v>
+      </c>
+      <c r="H33">
+        <v>44</v>
+      </c>
+      <c r="I33">
+        <v>34</v>
+      </c>
+      <c r="J33">
+        <v>44</v>
+      </c>
+      <c r="K33">
+        <v>44</v>
       </c>
       <c r="L33">
-        <v>23</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2276,37 +2287,37 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C34">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="D34">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E34">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F34">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G34">
         <v>48</v>
       </c>
       <c r="H34">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="I34">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="J34">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="K34">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="L34">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2314,113 +2325,113 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C35">
         <v>44</v>
       </c>
       <c r="D35">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="E35">
-        <v>49</v>
-      </c>
-      <c r="F35">
-        <v>46</v>
+        <v>36</v>
+      </c>
+      <c r="F35" t="s">
+        <v>5</v>
       </c>
       <c r="G35">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H35">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="I35">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="J35">
-        <v>50</v>
-      </c>
-      <c r="K35">
-        <v>53</v>
-      </c>
-      <c r="L35">
-        <v>69</v>
+        <v>34</v>
+      </c>
+      <c r="K35" t="s">
+        <v>5</v>
+      </c>
+      <c r="L35" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
-      <c r="B36">
-        <v>37</v>
-      </c>
-      <c r="C36">
-        <v>41</v>
-      </c>
-      <c r="D36">
-        <v>44</v>
-      </c>
-      <c r="E36">
-        <v>40</v>
-      </c>
-      <c r="F36">
-        <v>36</v>
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" t="s">
+        <v>5</v>
       </c>
       <c r="G36" t="s">
         <v>5</v>
       </c>
-      <c r="H36">
-        <v>43</v>
+      <c r="H36" t="s">
+        <v>5</v>
       </c>
       <c r="I36">
-        <v>36</v>
-      </c>
-      <c r="J36">
-        <v>38</v>
+        <v>23</v>
+      </c>
+      <c r="J36" t="s">
+        <v>5</v>
       </c>
       <c r="K36">
-        <v>34</v>
-      </c>
-      <c r="L36" t="s">
-        <v>5</v>
+        <v>14</v>
+      </c>
+      <c r="L36">
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" t="s">
-        <v>5</v>
-      </c>
-      <c r="F37" t="s">
-        <v>5</v>
-      </c>
-      <c r="G37" t="s">
-        <v>5</v>
-      </c>
-      <c r="H37" t="s">
-        <v>5</v>
-      </c>
-      <c r="I37" t="s">
-        <v>5</v>
+      <c r="B37">
+        <v>33</v>
+      </c>
+      <c r="C37">
+        <v>46</v>
+      </c>
+      <c r="D37">
+        <v>31</v>
+      </c>
+      <c r="E37">
+        <v>34</v>
+      </c>
+      <c r="F37">
+        <v>36</v>
+      </c>
+      <c r="G37">
+        <v>51</v>
+      </c>
+      <c r="H37">
+        <v>53</v>
+      </c>
+      <c r="I37">
+        <v>45</v>
       </c>
       <c r="J37">
-        <v>23</v>
-      </c>
-      <c r="K37" t="s">
-        <v>5</v>
+        <v>43</v>
+      </c>
+      <c r="K37">
+        <v>40</v>
       </c>
       <c r="L37">
-        <v>14</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2430,46 +2441,46 @@
       <c r="B38" t="s">
         <v>5</v>
       </c>
-      <c r="C38">
-        <v>33</v>
-      </c>
-      <c r="D38">
-        <v>46</v>
-      </c>
-      <c r="E38">
-        <v>31</v>
-      </c>
-      <c r="F38">
-        <v>34</v>
-      </c>
-      <c r="G38">
-        <v>36</v>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G38" t="s">
+        <v>5</v>
       </c>
       <c r="H38">
+        <v>43</v>
+      </c>
+      <c r="I38" t="s">
+        <v>5</v>
+      </c>
+      <c r="J38">
         <v>51</v>
       </c>
-      <c r="I38">
-        <v>53</v>
-      </c>
-      <c r="J38">
-        <v>45</v>
-      </c>
-      <c r="K38">
-        <v>43</v>
+      <c r="K38" t="s">
+        <v>5</v>
       </c>
       <c r="L38">
-        <v>40</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
-      <c r="B39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" t="s">
-        <v>5</v>
+      <c r="B39">
+        <v>48</v>
+      </c>
+      <c r="C39">
+        <v>41</v>
       </c>
       <c r="D39" t="s">
         <v>5</v>
@@ -2477,23 +2488,23 @@
       <c r="E39" t="s">
         <v>5</v>
       </c>
-      <c r="F39" t="s">
-        <v>5</v>
+      <c r="F39">
+        <v>68</v>
       </c>
       <c r="G39" t="s">
         <v>5</v>
       </c>
-      <c r="H39" t="s">
-        <v>5</v>
-      </c>
-      <c r="I39">
-        <v>43</v>
+      <c r="H39">
+        <v>74</v>
+      </c>
+      <c r="I39" t="s">
+        <v>5</v>
       </c>
       <c r="J39" t="s">
         <v>5</v>
       </c>
-      <c r="K39">
-        <v>51</v>
+      <c r="K39" t="s">
+        <v>5</v>
       </c>
       <c r="L39" t="s">
         <v>5</v>
@@ -2503,38 +2514,38 @@
       <c r="A40" t="s">
         <v>39</v>
       </c>
-      <c r="B40">
-        <v>55</v>
+      <c r="B40" t="s">
+        <v>5</v>
       </c>
       <c r="C40">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="D40">
-        <v>41</v>
-      </c>
-      <c r="E40" t="s">
-        <v>5</v>
-      </c>
-      <c r="F40" t="s">
-        <v>5</v>
+        <v>22</v>
+      </c>
+      <c r="E40">
+        <v>22</v>
+      </c>
+      <c r="F40">
+        <v>13</v>
       </c>
       <c r="G40">
-        <v>68</v>
-      </c>
-      <c r="H40" t="s">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="H40">
+        <v>31</v>
       </c>
       <c r="I40">
-        <v>74</v>
-      </c>
-      <c r="J40" t="s">
-        <v>5</v>
-      </c>
-      <c r="K40" t="s">
-        <v>5</v>
-      </c>
-      <c r="L40" t="s">
-        <v>5</v>
+        <v>27</v>
+      </c>
+      <c r="J40">
+        <v>47</v>
+      </c>
+      <c r="K40">
+        <v>36</v>
+      </c>
+      <c r="L40">
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -2542,83 +2553,83 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>28</v>
-      </c>
-      <c r="C41" t="s">
-        <v>5</v>
+        <v>45</v>
+      </c>
+      <c r="C41">
+        <v>47</v>
       </c>
       <c r="D41">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="E41">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="F41">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="G41">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="H41">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="I41">
-        <v>31</v>
-      </c>
-      <c r="J41">
-        <v>27</v>
-      </c>
-      <c r="K41">
-        <v>47</v>
-      </c>
-      <c r="L41">
-        <v>36</v>
+        <v>50</v>
+      </c>
+      <c r="J41" t="s">
+        <v>5</v>
+      </c>
+      <c r="K41" t="s">
+        <v>5</v>
+      </c>
+      <c r="L41" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
-      <c r="B42">
-        <v>48</v>
-      </c>
-      <c r="C42">
-        <v>45</v>
-      </c>
-      <c r="D42">
-        <v>47</v>
+      <c r="B42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>5</v>
       </c>
       <c r="E42">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="F42">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="G42">
-        <v>46</v>
-      </c>
-      <c r="H42">
-        <v>51</v>
-      </c>
-      <c r="I42">
-        <v>55</v>
-      </c>
-      <c r="J42">
-        <v>50</v>
+        <v>23</v>
+      </c>
+      <c r="H42" t="s">
+        <v>5</v>
+      </c>
+      <c r="I42" t="s">
+        <v>5</v>
+      </c>
+      <c r="J42" t="s">
+        <v>5</v>
       </c>
       <c r="K42" t="s">
         <v>5</v>
       </c>
-      <c r="L42" t="s">
-        <v>5</v>
+      <c r="L42">
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
-      <c r="B43">
-        <v>21</v>
+      <c r="B43" t="s">
+        <v>5</v>
       </c>
       <c r="C43" t="s">
         <v>5</v>
@@ -2626,29 +2637,29 @@
       <c r="D43" t="s">
         <v>5</v>
       </c>
-      <c r="E43" t="s">
-        <v>5</v>
-      </c>
-      <c r="F43">
-        <v>54</v>
-      </c>
-      <c r="G43">
-        <v>29</v>
-      </c>
-      <c r="H43">
+      <c r="E43">
+        <v>40</v>
+      </c>
+      <c r="F43" t="s">
+        <v>5</v>
+      </c>
+      <c r="G43" t="s">
+        <v>5</v>
+      </c>
+      <c r="H43" t="s">
+        <v>5</v>
+      </c>
+      <c r="I43" t="s">
+        <v>5</v>
+      </c>
+      <c r="J43" t="s">
+        <v>5</v>
+      </c>
+      <c r="K43" t="s">
+        <v>5</v>
+      </c>
+      <c r="L43">
         <v>23</v>
-      </c>
-      <c r="I43" t="s">
-        <v>5</v>
-      </c>
-      <c r="J43" t="s">
-        <v>5</v>
-      </c>
-      <c r="K43" t="s">
-        <v>5</v>
-      </c>
-      <c r="L43" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -2667,84 +2678,84 @@
       <c r="E44" t="s">
         <v>5</v>
       </c>
-      <c r="F44">
-        <v>40</v>
-      </c>
-      <c r="G44" t="s">
-        <v>5</v>
-      </c>
-      <c r="H44" t="s">
-        <v>5</v>
-      </c>
-      <c r="I44" t="s">
-        <v>5</v>
-      </c>
-      <c r="J44" t="s">
-        <v>5</v>
-      </c>
-      <c r="K44" t="s">
-        <v>5</v>
-      </c>
-      <c r="L44" t="s">
-        <v>5</v>
+      <c r="F44" t="s">
+        <v>5</v>
+      </c>
+      <c r="G44">
+        <v>24</v>
+      </c>
+      <c r="H44">
+        <v>53</v>
+      </c>
+      <c r="I44">
+        <v>38</v>
+      </c>
+      <c r="J44">
+        <v>16</v>
+      </c>
+      <c r="K44">
+        <v>11</v>
+      </c>
+      <c r="L44">
+        <v>27</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
-      <c r="B45" t="s">
-        <v>5</v>
-      </c>
-      <c r="C45" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" t="s">
-        <v>5</v>
-      </c>
-      <c r="E45" t="s">
-        <v>5</v>
-      </c>
-      <c r="F45" t="s">
-        <v>5</v>
-      </c>
-      <c r="G45" t="s">
-        <v>5</v>
-      </c>
-      <c r="H45">
-        <v>24</v>
+      <c r="B45">
+        <v>39</v>
+      </c>
+      <c r="C45">
+        <v>51</v>
+      </c>
+      <c r="D45">
+        <v>46</v>
+      </c>
+      <c r="E45">
+        <v>34</v>
+      </c>
+      <c r="F45">
+        <v>45</v>
+      </c>
+      <c r="G45">
+        <v>49</v>
+      </c>
+      <c r="H45" t="s">
+        <v>5</v>
       </c>
       <c r="I45">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J45">
-        <v>38</v>
-      </c>
-      <c r="K45">
-        <v>16</v>
-      </c>
-      <c r="L45">
-        <v>11</v>
+        <v>49</v>
+      </c>
+      <c r="K45" t="s">
+        <v>5</v>
+      </c>
+      <c r="L45" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
-      <c r="B46">
-        <v>31</v>
+      <c r="B46" t="s">
+        <v>5</v>
       </c>
       <c r="C46">
-        <v>39</v>
-      </c>
-      <c r="D46">
-        <v>51</v>
-      </c>
-      <c r="E46">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="D46" t="s">
+        <v>5</v>
+      </c>
+      <c r="E46" t="s">
+        <v>5</v>
       </c>
       <c r="F46">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="G46">
         <v>45</v>
@@ -2752,17 +2763,17 @@
       <c r="H46">
         <v>49</v>
       </c>
-      <c r="I46" t="s">
-        <v>5</v>
-      </c>
-      <c r="J46">
-        <v>52</v>
+      <c r="I46">
+        <v>43</v>
+      </c>
+      <c r="J46" t="s">
+        <v>5</v>
       </c>
       <c r="K46">
         <v>49</v>
       </c>
-      <c r="L46" t="s">
-        <v>5</v>
+      <c r="L46">
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -2770,151 +2781,151 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>34</v>
-      </c>
-      <c r="C47" t="s">
-        <v>5</v>
+        <v>57</v>
+      </c>
+      <c r="C47">
+        <v>57</v>
       </c>
       <c r="D47">
-        <v>45</v>
-      </c>
-      <c r="E47" t="s">
-        <v>5</v>
-      </c>
-      <c r="F47" t="s">
-        <v>5</v>
+        <v>31</v>
+      </c>
+      <c r="E47">
+        <v>52</v>
+      </c>
+      <c r="F47">
+        <v>50</v>
       </c>
       <c r="G47">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="H47">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="I47">
-        <v>49</v>
-      </c>
-      <c r="J47">
-        <v>43</v>
-      </c>
-      <c r="K47" t="s">
-        <v>5</v>
+        <v>40</v>
+      </c>
+      <c r="J47" t="s">
+        <v>5</v>
+      </c>
+      <c r="K47">
+        <v>79</v>
       </c>
       <c r="L47">
-        <v>49</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
-      <c r="B48">
-        <v>40</v>
-      </c>
-      <c r="C48">
-        <v>57</v>
+      <c r="B48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" t="s">
+        <v>5</v>
       </c>
       <c r="D48">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="E48">
-        <v>31</v>
-      </c>
-      <c r="F48">
-        <v>52</v>
+        <v>30</v>
+      </c>
+      <c r="F48" t="s">
+        <v>5</v>
       </c>
       <c r="G48">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="H48">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="I48">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="J48">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="K48" t="s">
         <v>5</v>
       </c>
       <c r="L48">
-        <v>79</v>
+        <v>25</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
-      <c r="B49" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" t="s">
-        <v>5</v>
+      <c r="B49">
+        <v>45</v>
+      </c>
+      <c r="C49">
+        <v>54</v>
+      </c>
+      <c r="D49">
+        <v>45</v>
       </c>
       <c r="E49">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="F49">
-        <v>30</v>
-      </c>
-      <c r="G49" t="s">
-        <v>5</v>
+        <v>48</v>
+      </c>
+      <c r="G49">
+        <v>48</v>
       </c>
       <c r="H49">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="I49">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="J49">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="K49">
-        <v>27</v>
-      </c>
-      <c r="L49" t="s">
-        <v>5</v>
+        <v>45</v>
+      </c>
+      <c r="L49">
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
-      <c r="B50">
-        <v>50</v>
+      <c r="B50" t="s">
+        <v>5</v>
       </c>
       <c r="C50">
+        <v>94</v>
+      </c>
+      <c r="D50" t="s">
+        <v>5</v>
+      </c>
+      <c r="E50" t="s">
+        <v>5</v>
+      </c>
+      <c r="F50" t="s">
+        <v>5</v>
+      </c>
+      <c r="G50" t="s">
+        <v>5</v>
+      </c>
+      <c r="H50">
         <v>45</v>
       </c>
-      <c r="D50">
-        <v>54</v>
-      </c>
-      <c r="E50">
-        <v>45</v>
-      </c>
-      <c r="F50">
-        <v>48</v>
-      </c>
-      <c r="G50">
-        <v>48</v>
-      </c>
-      <c r="H50">
-        <v>48</v>
-      </c>
-      <c r="I50">
-        <v>48</v>
-      </c>
-      <c r="J50">
-        <v>35</v>
-      </c>
-      <c r="K50">
-        <v>36</v>
-      </c>
-      <c r="L50">
-        <v>45</v>
+      <c r="I50" t="s">
+        <v>5</v>
+      </c>
+      <c r="J50" t="s">
+        <v>5</v>
+      </c>
+      <c r="K50" t="s">
+        <v>5</v>
+      </c>
+      <c r="L50" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -2927,14 +2938,14 @@
       <c r="C51" t="s">
         <v>5</v>
       </c>
-      <c r="D51">
-        <v>94</v>
+      <c r="D51" t="s">
+        <v>5</v>
       </c>
       <c r="E51" t="s">
         <v>5</v>
       </c>
-      <c r="F51" t="s">
-        <v>5</v>
+      <c r="F51">
+        <v>12</v>
       </c>
       <c r="G51" t="s">
         <v>5</v>
@@ -2942,8 +2953,8 @@
       <c r="H51" t="s">
         <v>5</v>
       </c>
-      <c r="I51">
-        <v>45</v>
+      <c r="I51" t="s">
+        <v>5</v>
       </c>
       <c r="J51" t="s">
         <v>5</v>
@@ -2975,57 +2986,57 @@
         <v>5</v>
       </c>
       <c r="G52">
-        <v>12</v>
-      </c>
-      <c r="H52" t="s">
-        <v>5</v>
-      </c>
-      <c r="I52" t="s">
-        <v>5</v>
-      </c>
-      <c r="J52" t="s">
-        <v>5</v>
-      </c>
-      <c r="K52" t="s">
-        <v>5</v>
-      </c>
-      <c r="L52" t="s">
-        <v>5</v>
+        <v>55</v>
+      </c>
+      <c r="H52">
+        <v>53</v>
+      </c>
+      <c r="I52">
+        <v>30</v>
+      </c>
+      <c r="J52">
+        <v>47</v>
+      </c>
+      <c r="K52">
+        <v>52</v>
+      </c>
+      <c r="L52">
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
-      <c r="B53">
-        <v>71</v>
+      <c r="B53" t="s">
+        <v>5</v>
       </c>
       <c r="C53" t="s">
         <v>5</v>
       </c>
-      <c r="D53" t="s">
-        <v>5</v>
-      </c>
-      <c r="E53" t="s">
-        <v>5</v>
-      </c>
-      <c r="F53" t="s">
-        <v>5</v>
-      </c>
-      <c r="G53" t="s">
-        <v>5</v>
+      <c r="D53">
+        <v>44</v>
+      </c>
+      <c r="E53">
+        <v>38</v>
+      </c>
+      <c r="F53">
+        <v>32</v>
+      </c>
+      <c r="G53">
+        <v>60</v>
       </c>
       <c r="H53">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="I53">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="J53">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="K53">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L53">
         <v>52</v>
@@ -3044,29 +3055,29 @@
       <c r="D54" t="s">
         <v>5</v>
       </c>
-      <c r="E54">
-        <v>44</v>
-      </c>
-      <c r="F54">
-        <v>38</v>
-      </c>
-      <c r="G54">
-        <v>32</v>
+      <c r="E54" t="s">
+        <v>5</v>
+      </c>
+      <c r="F54" t="s">
+        <v>5</v>
+      </c>
+      <c r="G54" t="s">
+        <v>5</v>
       </c>
       <c r="H54">
-        <v>60</v>
-      </c>
-      <c r="I54">
         <v>37</v>
       </c>
-      <c r="J54">
-        <v>45</v>
-      </c>
-      <c r="K54">
-        <v>52</v>
-      </c>
-      <c r="L54">
-        <v>49</v>
+      <c r="I54" t="s">
+        <v>5</v>
+      </c>
+      <c r="J54" t="s">
+        <v>5</v>
+      </c>
+      <c r="K54" t="s">
+        <v>5</v>
+      </c>
+      <c r="L54" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
@@ -3094,8 +3105,8 @@
       <c r="H55" t="s">
         <v>5</v>
       </c>
-      <c r="I55">
-        <v>37</v>
+      <c r="I55" t="s">
+        <v>5</v>
       </c>
       <c r="J55" t="s">
         <v>5</v>
@@ -3103,8 +3114,8 @@
       <c r="K55" t="s">
         <v>5</v>
       </c>
-      <c r="L55" t="s">
-        <v>5</v>
+      <c r="L55">
+        <v>47</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
@@ -3135,14 +3146,14 @@
       <c r="I56" t="s">
         <v>5</v>
       </c>
-      <c r="J56" t="s">
-        <v>5</v>
+      <c r="J56">
+        <v>37</v>
       </c>
       <c r="K56">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="L56">
-        <v>31</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
@@ -3167,20 +3178,20 @@
       <c r="G57" t="s">
         <v>5</v>
       </c>
-      <c r="H57">
-        <v>27</v>
+      <c r="H57" t="s">
+        <v>5</v>
       </c>
       <c r="I57" t="s">
         <v>5</v>
       </c>
-      <c r="J57">
-        <v>39</v>
+      <c r="J57" t="s">
+        <v>5</v>
       </c>
       <c r="K57" t="s">
         <v>5</v>
       </c>
       <c r="L57">
-        <v>38</v>
+        <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
@@ -3202,23 +3213,23 @@
       <c r="F58" t="s">
         <v>5</v>
       </c>
-      <c r="G58" t="s">
-        <v>5</v>
+      <c r="G58">
+        <v>27</v>
       </c>
       <c r="H58" t="s">
         <v>5</v>
       </c>
-      <c r="I58" t="s">
-        <v>5</v>
+      <c r="I58">
+        <v>39</v>
       </c>
       <c r="J58" t="s">
         <v>5</v>
       </c>
-      <c r="K58" t="s">
-        <v>5</v>
+      <c r="K58">
+        <v>38</v>
       </c>
       <c r="L58">
-        <v>66</v>
+        <v>26</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
@@ -3237,8 +3248,8 @@
       <c r="E59" t="s">
         <v>5</v>
       </c>
-      <c r="F59">
-        <v>52</v>
+      <c r="F59" t="s">
+        <v>5</v>
       </c>
       <c r="G59" t="s">
         <v>5</v>
@@ -3246,25 +3257,25 @@
       <c r="H59" t="s">
         <v>5</v>
       </c>
-      <c r="I59">
-        <v>35</v>
-      </c>
-      <c r="J59">
-        <v>14</v>
+      <c r="I59" t="s">
+        <v>5</v>
+      </c>
+      <c r="J59" t="s">
+        <v>5</v>
       </c>
       <c r="K59">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="L59">
-        <v>35</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
-      <c r="B60">
-        <v>60</v>
+      <c r="B60" t="s">
+        <v>5</v>
       </c>
       <c r="C60" t="s">
         <v>5</v>
@@ -3273,28 +3284,28 @@
         <v>5</v>
       </c>
       <c r="E60">
-        <v>45</v>
-      </c>
-      <c r="F60">
-        <v>54</v>
+        <v>52</v>
+      </c>
+      <c r="F60" t="s">
+        <v>5</v>
       </c>
       <c r="G60" t="s">
         <v>5</v>
       </c>
       <c r="H60">
-        <v>55</v>
-      </c>
-      <c r="I60" t="s">
-        <v>5</v>
+        <v>35</v>
+      </c>
+      <c r="I60">
+        <v>14</v>
       </c>
       <c r="J60">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="K60">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="L60">
-        <v>52</v>
+        <v>33</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
@@ -3307,32 +3318,32 @@
       <c r="C61" t="s">
         <v>5</v>
       </c>
-      <c r="D61" t="s">
-        <v>5</v>
-      </c>
-      <c r="E61" t="s">
-        <v>5</v>
+      <c r="D61">
+        <v>45</v>
+      </c>
+      <c r="E61">
+        <v>54</v>
       </c>
       <c r="F61" t="s">
         <v>5</v>
       </c>
-      <c r="G61" t="s">
-        <v>5</v>
+      <c r="G61">
+        <v>55</v>
       </c>
       <c r="H61" t="s">
         <v>5</v>
       </c>
-      <c r="I61" t="s">
-        <v>5</v>
+      <c r="I61">
+        <v>39</v>
       </c>
       <c r="J61">
-        <v>35</v>
-      </c>
-      <c r="K61" t="s">
-        <v>5</v>
-      </c>
-      <c r="L61" t="s">
-        <v>5</v>
+        <v>43</v>
+      </c>
+      <c r="K61">
+        <v>52</v>
+      </c>
+      <c r="L61">
+        <v>34</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
@@ -3361,7 +3372,7 @@
         <v>5</v>
       </c>
       <c r="I62">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="J62" t="s">
         <v>5</v>
@@ -3395,8 +3406,8 @@
       <c r="G63" t="s">
         <v>5</v>
       </c>
-      <c r="H63" t="s">
-        <v>5</v>
+      <c r="H63">
+        <v>17</v>
       </c>
       <c r="I63" t="s">
         <v>5</v>
@@ -3407,46 +3418,46 @@
       <c r="K63" t="s">
         <v>5</v>
       </c>
-      <c r="L63">
-        <v>62</v>
+      <c r="L63" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>63</v>
       </c>
-      <c r="B64">
-        <v>31</v>
-      </c>
-      <c r="C64">
-        <v>25</v>
-      </c>
-      <c r="D64">
-        <v>34</v>
-      </c>
-      <c r="E64">
-        <v>30</v>
-      </c>
-      <c r="F64">
-        <v>41</v>
-      </c>
-      <c r="G64">
-        <v>40</v>
-      </c>
-      <c r="H64">
-        <v>41</v>
-      </c>
-      <c r="I64">
-        <v>41</v>
-      </c>
-      <c r="J64">
-        <v>36</v>
+      <c r="B64" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" t="s">
+        <v>5</v>
+      </c>
+      <c r="E64" t="s">
+        <v>5</v>
+      </c>
+      <c r="F64" t="s">
+        <v>5</v>
+      </c>
+      <c r="G64" t="s">
+        <v>5</v>
+      </c>
+      <c r="H64" t="s">
+        <v>5</v>
+      </c>
+      <c r="I64" t="s">
+        <v>5</v>
+      </c>
+      <c r="J64" t="s">
+        <v>5</v>
       </c>
       <c r="K64">
-        <v>52</v>
-      </c>
-      <c r="L64">
-        <v>42</v>
+        <v>62</v>
+      </c>
+      <c r="L64" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
@@ -3454,51 +3465,51 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C65">
         <v>34</v>
       </c>
       <c r="D65">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="E65">
-        <v>38</v>
-      </c>
-      <c r="F65" t="s">
-        <v>5</v>
-      </c>
-      <c r="G65" t="s">
-        <v>5</v>
-      </c>
-      <c r="H65" t="s">
-        <v>5</v>
-      </c>
-      <c r="I65" t="s">
-        <v>5</v>
-      </c>
-      <c r="J65" t="s">
-        <v>5</v>
-      </c>
-      <c r="K65" t="s">
-        <v>5</v>
-      </c>
-      <c r="L65" t="s">
-        <v>5</v>
+        <v>41</v>
+      </c>
+      <c r="F65">
+        <v>40</v>
+      </c>
+      <c r="G65">
+        <v>41</v>
+      </c>
+      <c r="H65">
+        <v>41</v>
+      </c>
+      <c r="I65">
+        <v>36</v>
+      </c>
+      <c r="J65">
+        <v>52</v>
+      </c>
+      <c r="K65">
+        <v>42</v>
+      </c>
+      <c r="L65">
+        <v>44</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>65</v>
       </c>
-      <c r="B66" t="s">
-        <v>5</v>
-      </c>
-      <c r="C66" t="s">
-        <v>5</v>
-      </c>
-      <c r="D66" t="s">
-        <v>5</v>
+      <c r="B66">
+        <v>34</v>
+      </c>
+      <c r="C66">
+        <v>13</v>
+      </c>
+      <c r="D66">
+        <v>38</v>
       </c>
       <c r="E66" t="s">
         <v>5</v>
@@ -3521,84 +3532,84 @@
       <c r="K66" t="s">
         <v>5</v>
       </c>
-      <c r="L66">
-        <v>36</v>
+      <c r="L66" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>66</v>
       </c>
-      <c r="B67">
+      <c r="B67" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" t="s">
+        <v>5</v>
+      </c>
+      <c r="E67" t="s">
+        <v>5</v>
+      </c>
+      <c r="F67" t="s">
+        <v>5</v>
+      </c>
+      <c r="G67" t="s">
+        <v>5</v>
+      </c>
+      <c r="H67" t="s">
+        <v>5</v>
+      </c>
+      <c r="I67" t="s">
+        <v>5</v>
+      </c>
+      <c r="J67" t="s">
+        <v>5</v>
+      </c>
+      <c r="K67">
+        <v>36</v>
+      </c>
+      <c r="L67">
         <v>32</v>
-      </c>
-      <c r="C67">
-        <v>42</v>
-      </c>
-      <c r="D67">
-        <v>44</v>
-      </c>
-      <c r="E67">
-        <v>40</v>
-      </c>
-      <c r="F67">
-        <v>46</v>
-      </c>
-      <c r="G67">
-        <v>26</v>
-      </c>
-      <c r="H67">
-        <v>42</v>
-      </c>
-      <c r="I67">
-        <v>49</v>
-      </c>
-      <c r="J67" t="s">
-        <v>5</v>
-      </c>
-      <c r="K67">
-        <v>35</v>
-      </c>
-      <c r="L67">
-        <v>28</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>67</v>
       </c>
-      <c r="B68" t="s">
-        <v>5</v>
-      </c>
-      <c r="C68" t="s">
-        <v>5</v>
-      </c>
-      <c r="D68" t="s">
-        <v>5</v>
-      </c>
-      <c r="E68" t="s">
-        <v>5</v>
-      </c>
-      <c r="F68" t="s">
-        <v>5</v>
-      </c>
-      <c r="G68" t="s">
-        <v>5</v>
-      </c>
-      <c r="H68" t="s">
-        <v>5</v>
+      <c r="B68">
+        <v>42</v>
+      </c>
+      <c r="C68">
+        <v>44</v>
+      </c>
+      <c r="D68">
+        <v>40</v>
+      </c>
+      <c r="E68">
+        <v>46</v>
+      </c>
+      <c r="F68">
+        <v>26</v>
+      </c>
+      <c r="G68">
+        <v>42</v>
+      </c>
+      <c r="H68">
+        <v>49</v>
       </c>
       <c r="I68" t="s">
         <v>5</v>
       </c>
-      <c r="J68" t="s">
-        <v>5</v>
+      <c r="J68">
+        <v>35</v>
       </c>
       <c r="K68">
-        <v>43</v>
-      </c>
-      <c r="L68" t="s">
-        <v>5</v>
+        <v>28</v>
+      </c>
+      <c r="L68">
+        <v>26</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
@@ -3626,17 +3637,17 @@
       <c r="H69" t="s">
         <v>5</v>
       </c>
-      <c r="I69">
-        <v>22</v>
+      <c r="I69" t="s">
+        <v>5</v>
       </c>
       <c r="J69">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="K69" t="s">
         <v>5</v>
       </c>
-      <c r="L69">
-        <v>48</v>
+      <c r="L69" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
@@ -3661,20 +3672,20 @@
       <c r="G70" t="s">
         <v>5</v>
       </c>
-      <c r="H70" t="s">
-        <v>5</v>
+      <c r="H70">
+        <v>22</v>
       </c>
       <c r="I70">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="J70" t="s">
         <v>5</v>
       </c>
       <c r="K70">
-        <v>56</v>
-      </c>
-      <c r="L70">
-        <v>36</v>
+        <v>48</v>
+      </c>
+      <c r="L70" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
@@ -3687,32 +3698,32 @@
       <c r="C71" t="s">
         <v>5</v>
       </c>
-      <c r="D71">
-        <v>66</v>
+      <c r="D71" t="s">
+        <v>5</v>
       </c>
       <c r="E71" t="s">
         <v>5</v>
       </c>
-      <c r="F71">
-        <v>79</v>
-      </c>
-      <c r="G71">
-        <v>74</v>
+      <c r="F71" t="s">
+        <v>5</v>
+      </c>
+      <c r="G71" t="s">
+        <v>5</v>
       </c>
       <c r="H71">
-        <v>77</v>
-      </c>
-      <c r="I71">
-        <v>78</v>
+        <v>28</v>
+      </c>
+      <c r="I71" t="s">
+        <v>5</v>
       </c>
       <c r="J71">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="K71">
-        <v>79</v>
+        <v>36</v>
       </c>
       <c r="L71">
-        <v>43</v>
+        <v>24</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
@@ -3722,52 +3733,52 @@
       <c r="B72" t="s">
         <v>5</v>
       </c>
-      <c r="C72" t="s">
-        <v>5</v>
+      <c r="C72">
+        <v>66</v>
       </c>
       <c r="D72" t="s">
         <v>5</v>
       </c>
-      <c r="E72" t="s">
-        <v>5</v>
+      <c r="E72">
+        <v>79</v>
       </c>
       <c r="F72">
-        <v>28</v>
-      </c>
-      <c r="G72" t="s">
-        <v>5</v>
-      </c>
-      <c r="H72" t="s">
-        <v>5</v>
-      </c>
-      <c r="I72" t="s">
-        <v>5</v>
-      </c>
-      <c r="J72" t="s">
-        <v>5</v>
-      </c>
-      <c r="K72" t="s">
-        <v>5</v>
-      </c>
-      <c r="L72" t="s">
-        <v>5</v>
+        <v>74</v>
+      </c>
+      <c r="G72">
+        <v>77</v>
+      </c>
+      <c r="H72">
+        <v>78</v>
+      </c>
+      <c r="I72">
+        <v>80</v>
+      </c>
+      <c r="J72">
+        <v>79</v>
+      </c>
+      <c r="K72">
+        <v>43</v>
+      </c>
+      <c r="L72">
+        <v>36</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>72</v>
       </c>
-      <c r="B73">
-        <v>29</v>
+      <c r="B73" t="s">
+        <v>5</v>
       </c>
       <c r="C73" t="s">
         <v>5</v>
       </c>
-      <c r="D73">
-        <v>43</v>
-      </c>
-      <c r="E73" t="s">
-        <v>5</v>
+      <c r="D73" t="s">
+        <v>5</v>
+      </c>
+      <c r="E73">
+        <v>28</v>
       </c>
       <c r="F73" t="s">
         <v>5</v>
@@ -3784,11 +3795,11 @@
       <c r="J73" t="s">
         <v>5</v>
       </c>
-      <c r="K73">
-        <v>75</v>
+      <c r="K73" t="s">
+        <v>5</v>
       </c>
       <c r="L73">
-        <v>72</v>
+        <v>55</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
@@ -3798,11 +3809,11 @@
       <c r="B74" t="s">
         <v>5</v>
       </c>
-      <c r="C74" t="s">
-        <v>5</v>
-      </c>
-      <c r="D74">
-        <v>31</v>
+      <c r="C74">
+        <v>43</v>
+      </c>
+      <c r="D74" t="s">
+        <v>5</v>
       </c>
       <c r="E74" t="s">
         <v>5</v>
@@ -3810,8 +3821,8 @@
       <c r="F74" t="s">
         <v>5</v>
       </c>
-      <c r="G74">
-        <v>36</v>
+      <c r="G74" t="s">
+        <v>5</v>
       </c>
       <c r="H74" t="s">
         <v>5</v>
@@ -3820,13 +3831,13 @@
         <v>5</v>
       </c>
       <c r="J74">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="K74">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="L74">
-        <v>43</v>
+        <v>65</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
@@ -3836,8 +3847,8 @@
       <c r="B75" t="s">
         <v>5</v>
       </c>
-      <c r="C75" t="s">
-        <v>5</v>
+      <c r="C75">
+        <v>31</v>
       </c>
       <c r="D75" t="s">
         <v>5</v>
@@ -3845,26 +3856,26 @@
       <c r="E75" t="s">
         <v>5</v>
       </c>
-      <c r="F75" t="s">
-        <v>5</v>
-      </c>
-      <c r="G75">
-        <v>71</v>
+      <c r="F75">
+        <v>36</v>
+      </c>
+      <c r="G75" t="s">
+        <v>5</v>
       </c>
       <c r="H75" t="s">
         <v>5</v>
       </c>
-      <c r="I75" t="s">
-        <v>5</v>
-      </c>
-      <c r="J75" t="s">
-        <v>5</v>
-      </c>
-      <c r="K75" t="s">
-        <v>5</v>
-      </c>
-      <c r="L75" t="s">
-        <v>5</v>
+      <c r="I75">
+        <v>28</v>
+      </c>
+      <c r="J75">
+        <v>32</v>
+      </c>
+      <c r="K75">
+        <v>43</v>
+      </c>
+      <c r="L75">
+        <v>46</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
@@ -3883,34 +3894,34 @@
       <c r="E76" t="s">
         <v>5</v>
       </c>
-      <c r="F76" t="s">
-        <v>5</v>
-      </c>
-      <c r="G76">
-        <v>36</v>
-      </c>
-      <c r="H76">
-        <v>34</v>
-      </c>
-      <c r="I76">
-        <v>39</v>
-      </c>
-      <c r="J76">
-        <v>29</v>
-      </c>
-      <c r="K76">
-        <v>43</v>
+      <c r="F76">
+        <v>71</v>
+      </c>
+      <c r="G76" t="s">
+        <v>5</v>
+      </c>
+      <c r="H76" t="s">
+        <v>5</v>
+      </c>
+      <c r="I76" t="s">
+        <v>5</v>
+      </c>
+      <c r="J76" t="s">
+        <v>5</v>
+      </c>
+      <c r="K76" t="s">
+        <v>5</v>
       </c>
       <c r="L76">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>76</v>
       </c>
-      <c r="B77">
-        <v>21</v>
+      <c r="B77" t="s">
+        <v>5</v>
       </c>
       <c r="C77" t="s">
         <v>5</v>
@@ -3922,25 +3933,25 @@
         <v>5</v>
       </c>
       <c r="F77">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G77">
+        <v>34</v>
+      </c>
+      <c r="H77">
         <v>39</v>
       </c>
-      <c r="H77">
-        <v>35</v>
-      </c>
       <c r="I77">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="J77">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="K77">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="L77">
-        <v>27</v>
+        <v>47</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
@@ -3956,29 +3967,29 @@
       <c r="D78" t="s">
         <v>5</v>
       </c>
-      <c r="E78" t="s">
-        <v>5</v>
-      </c>
-      <c r="F78" t="s">
-        <v>5</v>
-      </c>
-      <c r="G78" t="s">
-        <v>5</v>
-      </c>
-      <c r="H78" t="s">
-        <v>5</v>
+      <c r="E78">
+        <v>38</v>
+      </c>
+      <c r="F78">
+        <v>39</v>
+      </c>
+      <c r="G78">
+        <v>35</v>
+      </c>
+      <c r="H78">
+        <v>42</v>
       </c>
       <c r="I78">
-        <v>72</v>
-      </c>
-      <c r="J78" t="s">
-        <v>5</v>
-      </c>
-      <c r="K78" t="s">
-        <v>5</v>
-      </c>
-      <c r="L78" t="s">
-        <v>5</v>
+        <v>36</v>
+      </c>
+      <c r="J78">
+        <v>29</v>
+      </c>
+      <c r="K78">
+        <v>27</v>
+      </c>
+      <c r="L78">
+        <v>29</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
@@ -4000,14 +4011,14 @@
       <c r="F79" t="s">
         <v>5</v>
       </c>
-      <c r="G79">
-        <v>18</v>
+      <c r="G79" t="s">
+        <v>5</v>
       </c>
       <c r="H79">
-        <v>24</v>
-      </c>
-      <c r="I79">
-        <v>43</v>
+        <v>72</v>
+      </c>
+      <c r="I79" t="s">
+        <v>5</v>
       </c>
       <c r="J79" t="s">
         <v>5</v>
@@ -4023,26 +4034,26 @@
       <c r="A80" t="s">
         <v>79</v>
       </c>
-      <c r="B80">
-        <v>36</v>
-      </c>
-      <c r="C80">
-        <v>48</v>
-      </c>
-      <c r="D80">
-        <v>38</v>
-      </c>
-      <c r="E80">
-        <v>37</v>
+      <c r="B80" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" t="s">
+        <v>5</v>
+      </c>
+      <c r="D80" t="s">
+        <v>5</v>
+      </c>
+      <c r="E80" t="s">
+        <v>5</v>
       </c>
       <c r="F80">
-        <v>47</v>
-      </c>
-      <c r="G80" t="s">
-        <v>5</v>
-      </c>
-      <c r="H80" t="s">
-        <v>5</v>
+        <v>18</v>
+      </c>
+      <c r="G80">
+        <v>24</v>
+      </c>
+      <c r="H80">
+        <v>43</v>
       </c>
       <c r="I80" t="s">
         <v>5</v>
@@ -4050,8 +4061,8 @@
       <c r="J80" t="s">
         <v>5</v>
       </c>
-      <c r="K80">
-        <v>40</v>
+      <c r="K80" t="s">
+        <v>5</v>
       </c>
       <c r="L80" t="s">
         <v>5</v>
@@ -4061,17 +4072,17 @@
       <c r="A81" t="s">
         <v>80</v>
       </c>
-      <c r="B81" t="s">
-        <v>5</v>
-      </c>
-      <c r="C81" t="s">
-        <v>5</v>
-      </c>
-      <c r="D81" t="s">
-        <v>5</v>
-      </c>
-      <c r="E81" t="s">
-        <v>5</v>
+      <c r="B81">
+        <v>48</v>
+      </c>
+      <c r="C81">
+        <v>38</v>
+      </c>
+      <c r="D81">
+        <v>37</v>
+      </c>
+      <c r="E81">
+        <v>47</v>
       </c>
       <c r="F81" t="s">
         <v>5</v>
@@ -4085,52 +4096,52 @@
       <c r="I81" t="s">
         <v>5</v>
       </c>
-      <c r="J81" t="s">
-        <v>5</v>
-      </c>
-      <c r="K81">
-        <v>42</v>
-      </c>
-      <c r="L81">
-        <v>52</v>
+      <c r="J81">
+        <v>40</v>
+      </c>
+      <c r="K81" t="s">
+        <v>5</v>
+      </c>
+      <c r="L81" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>81</v>
       </c>
-      <c r="B82">
-        <v>48</v>
-      </c>
-      <c r="C82">
-        <v>58</v>
-      </c>
-      <c r="D82">
-        <v>59</v>
-      </c>
-      <c r="E82">
-        <v>48</v>
-      </c>
-      <c r="F82">
-        <v>55</v>
-      </c>
-      <c r="G82">
-        <v>49</v>
-      </c>
-      <c r="H82">
-        <v>47</v>
-      </c>
-      <c r="I82">
-        <v>49</v>
+      <c r="B82" t="s">
+        <v>5</v>
+      </c>
+      <c r="C82" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" t="s">
+        <v>5</v>
+      </c>
+      <c r="E82" t="s">
+        <v>5</v>
+      </c>
+      <c r="F82" t="s">
+        <v>5</v>
+      </c>
+      <c r="G82" t="s">
+        <v>5</v>
+      </c>
+      <c r="H82" t="s">
+        <v>5</v>
+      </c>
+      <c r="I82" t="s">
+        <v>5</v>
       </c>
       <c r="J82">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="K82">
+        <v>52</v>
+      </c>
+      <c r="L82">
         <v>51</v>
-      </c>
-      <c r="L82">
-        <v>49</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
@@ -4138,37 +4149,37 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="C83">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D83">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E83">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="F83">
-        <v>44</v>
-      </c>
-      <c r="G83" t="s">
-        <v>5</v>
+        <v>49</v>
+      </c>
+      <c r="G83">
+        <v>47</v>
       </c>
       <c r="H83">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="I83">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J83">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="K83">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L83">
-        <v>66</v>
+        <v>48</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
@@ -4179,34 +4190,34 @@
         <v>53</v>
       </c>
       <c r="C84">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D84">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E84">
-        <v>41</v>
-      </c>
-      <c r="F84">
-        <v>48</v>
+        <v>44</v>
+      </c>
+      <c r="F84" t="s">
+        <v>5</v>
       </c>
       <c r="G84">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="H84">
+        <v>57</v>
+      </c>
+      <c r="I84">
+        <v>59</v>
+      </c>
+      <c r="J84">
         <v>51</v>
       </c>
-      <c r="I84">
-        <v>37</v>
-      </c>
-      <c r="J84">
-        <v>31</v>
-      </c>
       <c r="K84">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="L84">
-        <v>42</v>
+        <v>68</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
@@ -4214,95 +4225,95 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C85">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D85">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="E85">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="F85">
         <v>49</v>
       </c>
       <c r="G85">
-        <v>30</v>
-      </c>
-      <c r="H85" t="s">
-        <v>5</v>
-      </c>
-      <c r="I85" t="s">
-        <v>5</v>
+        <v>51</v>
+      </c>
+      <c r="H85">
+        <v>37</v>
+      </c>
+      <c r="I85">
+        <v>31</v>
       </c>
       <c r="J85">
+        <v>36</v>
+      </c>
+      <c r="K85">
         <v>42</v>
       </c>
-      <c r="K85">
-        <v>41</v>
-      </c>
       <c r="L85">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>85</v>
       </c>
-      <c r="B86">
-        <v>50</v>
-      </c>
-      <c r="C86">
-        <v>39</v>
+      <c r="B86" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" t="s">
+        <v>5</v>
       </c>
       <c r="D86" t="s">
         <v>5</v>
       </c>
-      <c r="E86">
-        <v>42</v>
+      <c r="E86" t="s">
+        <v>5</v>
       </c>
       <c r="F86" t="s">
         <v>5</v>
       </c>
-      <c r="G86">
-        <v>48</v>
+      <c r="G86" t="s">
+        <v>5</v>
       </c>
       <c r="H86" t="s">
         <v>5</v>
       </c>
-      <c r="I86">
-        <v>46</v>
-      </c>
-      <c r="J86">
-        <v>50</v>
-      </c>
-      <c r="K86">
-        <v>45</v>
+      <c r="I86" t="s">
+        <v>5</v>
+      </c>
+      <c r="J86" t="s">
+        <v>5</v>
+      </c>
+      <c r="K86" t="s">
+        <v>5</v>
       </c>
       <c r="L86">
-        <v>43</v>
+        <v>23</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>86</v>
       </c>
-      <c r="B87" t="s">
-        <v>5</v>
-      </c>
-      <c r="C87" t="s">
-        <v>5</v>
-      </c>
-      <c r="D87" t="s">
-        <v>5</v>
-      </c>
-      <c r="E87" t="s">
-        <v>5</v>
-      </c>
-      <c r="F87" t="s">
-        <v>5</v>
+      <c r="B87">
+        <v>35</v>
+      </c>
+      <c r="C87">
+        <v>36</v>
+      </c>
+      <c r="D87">
+        <v>29</v>
+      </c>
+      <c r="E87">
+        <v>49</v>
+      </c>
+      <c r="F87">
+        <v>30</v>
       </c>
       <c r="G87" t="s">
         <v>5</v>
@@ -4311,16 +4322,16 @@
         <v>5</v>
       </c>
       <c r="I87">
-        <v>43</v>
-      </c>
-      <c r="J87" t="s">
-        <v>5</v>
-      </c>
-      <c r="K87" t="s">
-        <v>5</v>
-      </c>
-      <c r="L87" t="s">
-        <v>5</v>
+        <v>42</v>
+      </c>
+      <c r="J87">
+        <v>41</v>
+      </c>
+      <c r="K87">
+        <v>36</v>
+      </c>
+      <c r="L87">
+        <v>46</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
@@ -4328,45 +4339,45 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C88" t="s">
         <v>5</v>
       </c>
-      <c r="D88" t="s">
-        <v>5</v>
+      <c r="D88">
+        <v>42</v>
       </c>
       <c r="E88" t="s">
         <v>5</v>
       </c>
-      <c r="F88" t="s">
-        <v>5</v>
+      <c r="F88">
+        <v>48</v>
       </c>
       <c r="G88" t="s">
         <v>5</v>
       </c>
-      <c r="H88" t="s">
-        <v>5</v>
-      </c>
-      <c r="I88" t="s">
-        <v>5</v>
+      <c r="H88">
+        <v>46</v>
+      </c>
+      <c r="I88">
+        <v>50</v>
       </c>
       <c r="J88">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="K88">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="L88">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>88</v>
       </c>
-      <c r="B89">
-        <v>47</v>
+      <c r="B89" t="s">
+        <v>5</v>
       </c>
       <c r="C89" t="s">
         <v>5</v>
@@ -4374,17 +4385,17 @@
       <c r="D89" t="s">
         <v>5</v>
       </c>
-      <c r="E89">
-        <v>63</v>
-      </c>
-      <c r="F89">
-        <v>50</v>
-      </c>
-      <c r="G89">
-        <v>42</v>
-      </c>
-      <c r="H89" t="s">
-        <v>5</v>
+      <c r="E89" t="s">
+        <v>5</v>
+      </c>
+      <c r="F89" t="s">
+        <v>5</v>
+      </c>
+      <c r="G89" t="s">
+        <v>5</v>
+      </c>
+      <c r="H89">
+        <v>43</v>
       </c>
       <c r="I89" t="s">
         <v>5</v>
@@ -4392,11 +4403,11 @@
       <c r="J89" t="s">
         <v>5</v>
       </c>
-      <c r="K89">
-        <v>58</v>
-      </c>
-      <c r="L89">
-        <v>42</v>
+      <c r="K89" t="s">
+        <v>5</v>
+      </c>
+      <c r="L89" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
@@ -4425,16 +4436,16 @@
         <v>5</v>
       </c>
       <c r="I90">
-        <v>52</v>
-      </c>
-      <c r="J90" t="s">
-        <v>5</v>
-      </c>
-      <c r="K90" t="s">
-        <v>5</v>
-      </c>
-      <c r="L90" t="s">
-        <v>5</v>
+        <v>66</v>
+      </c>
+      <c r="J90">
+        <v>70</v>
+      </c>
+      <c r="K90">
+        <v>63</v>
+      </c>
+      <c r="L90">
+        <v>72</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
@@ -4447,14 +4458,14 @@
       <c r="C91" t="s">
         <v>5</v>
       </c>
-      <c r="D91" t="s">
-        <v>5</v>
-      </c>
-      <c r="E91" t="s">
-        <v>5</v>
-      </c>
-      <c r="F91" t="s">
-        <v>5</v>
+      <c r="D91">
+        <v>63</v>
+      </c>
+      <c r="E91">
+        <v>50</v>
+      </c>
+      <c r="F91">
+        <v>42</v>
       </c>
       <c r="G91" t="s">
         <v>5</v>
@@ -4466,13 +4477,13 @@
         <v>5</v>
       </c>
       <c r="J91">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="K91">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="L91">
-        <v>22</v>
+        <v>59</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
@@ -4497,20 +4508,20 @@
       <c r="G92" t="s">
         <v>5</v>
       </c>
-      <c r="H92" t="s">
-        <v>5</v>
-      </c>
-      <c r="I92">
-        <v>25</v>
-      </c>
-      <c r="J92">
-        <v>37</v>
+      <c r="H92">
+        <v>52</v>
+      </c>
+      <c r="I92" t="s">
+        <v>5</v>
+      </c>
+      <c r="J92" t="s">
+        <v>5</v>
       </c>
       <c r="K92" t="s">
         <v>5</v>
       </c>
-      <c r="L92">
-        <v>52</v>
+      <c r="L92" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
@@ -4529,26 +4540,26 @@
       <c r="E93" t="s">
         <v>5</v>
       </c>
-      <c r="F93">
-        <v>65</v>
-      </c>
-      <c r="G93">
-        <v>70</v>
-      </c>
-      <c r="H93">
-        <v>87</v>
-      </c>
-      <c r="I93" t="s">
-        <v>5</v>
-      </c>
-      <c r="J93" t="s">
-        <v>5</v>
+      <c r="F93" t="s">
+        <v>5</v>
+      </c>
+      <c r="G93" t="s">
+        <v>5</v>
+      </c>
+      <c r="H93" t="s">
+        <v>5</v>
+      </c>
+      <c r="I93">
+        <v>13</v>
+      </c>
+      <c r="J93">
+        <v>11</v>
       </c>
       <c r="K93">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="L93">
-        <v>60</v>
+        <v>17</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
@@ -4558,11 +4569,11 @@
       <c r="B94" t="s">
         <v>5</v>
       </c>
-      <c r="C94">
-        <v>24</v>
-      </c>
-      <c r="D94">
-        <v>29</v>
+      <c r="C94" t="s">
+        <v>5</v>
+      </c>
+      <c r="D94" t="s">
+        <v>5</v>
       </c>
       <c r="E94" t="s">
         <v>5</v>
@@ -4573,20 +4584,20 @@
       <c r="G94" t="s">
         <v>5</v>
       </c>
-      <c r="H94" t="s">
-        <v>5</v>
+      <c r="H94">
+        <v>25</v>
       </c>
       <c r="I94">
-        <v>16</v>
-      </c>
-      <c r="J94">
-        <v>29</v>
-      </c>
-      <c r="K94" t="s">
-        <v>5</v>
-      </c>
-      <c r="L94">
-        <v>16</v>
+        <v>37</v>
+      </c>
+      <c r="J94" t="s">
+        <v>5</v>
+      </c>
+      <c r="K94">
+        <v>52</v>
+      </c>
+      <c r="L94" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
@@ -4602,26 +4613,26 @@
       <c r="D95" t="s">
         <v>5</v>
       </c>
-      <c r="E95" t="s">
-        <v>5</v>
+      <c r="E95">
+        <v>65</v>
       </c>
       <c r="F95">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="G95">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="H95" t="s">
         <v>5</v>
       </c>
-      <c r="I95">
-        <v>62</v>
-      </c>
-      <c r="J95" t="s">
-        <v>5</v>
+      <c r="I95" t="s">
+        <v>5</v>
+      </c>
+      <c r="J95">
+        <v>68</v>
       </c>
       <c r="K95">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="L95" t="s">
         <v>5</v>
@@ -4632,151 +4643,151 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C96">
-        <v>40</v>
-      </c>
-      <c r="D96">
-        <v>42</v>
-      </c>
-      <c r="E96">
-        <v>42</v>
-      </c>
-      <c r="F96">
-        <v>38</v>
-      </c>
-      <c r="G96">
-        <v>35</v>
+        <v>29</v>
+      </c>
+      <c r="D96" t="s">
+        <v>5</v>
+      </c>
+      <c r="E96" t="s">
+        <v>5</v>
+      </c>
+      <c r="F96" t="s">
+        <v>5</v>
+      </c>
+      <c r="G96" t="s">
+        <v>5</v>
       </c>
       <c r="H96">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="I96">
-        <v>36</v>
-      </c>
-      <c r="J96">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="J96" t="s">
+        <v>5</v>
       </c>
       <c r="K96">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="L96">
-        <v>38</v>
+        <v>15</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>96</v>
       </c>
-      <c r="B97">
-        <v>45</v>
-      </c>
-      <c r="C97">
-        <v>38</v>
-      </c>
-      <c r="D97">
-        <v>37</v>
+      <c r="B97" t="s">
+        <v>5</v>
+      </c>
+      <c r="C97" t="s">
+        <v>5</v>
+      </c>
+      <c r="D97" t="s">
+        <v>5</v>
       </c>
       <c r="E97">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="F97">
-        <v>39</v>
-      </c>
-      <c r="G97">
-        <v>49</v>
+        <v>84</v>
+      </c>
+      <c r="G97" t="s">
+        <v>5</v>
       </c>
       <c r="H97">
-        <v>40</v>
-      </c>
-      <c r="I97">
-        <v>37</v>
+        <v>62</v>
+      </c>
+      <c r="I97" t="s">
+        <v>5</v>
       </c>
       <c r="J97">
-        <v>32</v>
-      </c>
-      <c r="K97">
-        <v>45</v>
-      </c>
-      <c r="L97">
-        <v>47</v>
+        <v>57</v>
+      </c>
+      <c r="K97" t="s">
+        <v>5</v>
+      </c>
+      <c r="L97" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>97</v>
       </c>
-      <c r="B98" t="s">
-        <v>5</v>
-      </c>
-      <c r="C98" t="s">
-        <v>5</v>
-      </c>
-      <c r="D98" t="s">
-        <v>5</v>
-      </c>
-      <c r="E98" t="s">
-        <v>5</v>
+      <c r="B98">
+        <v>40</v>
+      </c>
+      <c r="C98">
+        <v>42</v>
+      </c>
+      <c r="D98">
+        <v>42</v>
+      </c>
+      <c r="E98">
+        <v>38</v>
       </c>
       <c r="F98">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="G98">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="H98">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="I98">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="J98">
         <v>52</v>
       </c>
       <c r="K98">
-        <v>30</v>
-      </c>
-      <c r="L98" t="s">
-        <v>5</v>
+        <v>38</v>
+      </c>
+      <c r="L98">
+        <v>43</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>98</v>
       </c>
-      <c r="B99" t="s">
-        <v>5</v>
-      </c>
-      <c r="C99" t="s">
-        <v>5</v>
-      </c>
-      <c r="D99" t="s">
-        <v>5</v>
-      </c>
-      <c r="E99" t="s">
-        <v>5</v>
-      </c>
-      <c r="F99" t="s">
-        <v>5</v>
-      </c>
-      <c r="G99" t="s">
-        <v>5</v>
-      </c>
-      <c r="H99" t="s">
-        <v>5</v>
-      </c>
-      <c r="I99" t="s">
-        <v>5</v>
+      <c r="B99">
+        <v>38</v>
+      </c>
+      <c r="C99">
+        <v>37</v>
+      </c>
+      <c r="D99">
+        <v>39</v>
+      </c>
+      <c r="E99">
+        <v>39</v>
+      </c>
+      <c r="F99">
+        <v>49</v>
+      </c>
+      <c r="G99">
+        <v>40</v>
+      </c>
+      <c r="H99">
+        <v>37</v>
+      </c>
+      <c r="I99">
+        <v>32</v>
       </c>
       <c r="J99">
-        <v>44</v>
-      </c>
-      <c r="K99" t="s">
-        <v>5</v>
-      </c>
-      <c r="L99" t="s">
-        <v>5</v>
+        <v>45</v>
+      </c>
+      <c r="K99">
+        <v>47</v>
+      </c>
+      <c r="L99">
+        <v>45</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
@@ -4786,32 +4797,32 @@
       <c r="B100" t="s">
         <v>5</v>
       </c>
-      <c r="C100">
-        <v>25</v>
+      <c r="C100" t="s">
+        <v>5</v>
       </c>
       <c r="D100" t="s">
         <v>5</v>
       </c>
       <c r="E100">
-        <v>26</v>
-      </c>
-      <c r="F100" t="s">
-        <v>5</v>
+        <v>60</v>
+      </c>
+      <c r="F100">
+        <v>63</v>
       </c>
       <c r="G100">
-        <v>24</v>
-      </c>
-      <c r="H100" t="s">
-        <v>5</v>
+        <v>66</v>
+      </c>
+      <c r="H100">
+        <v>62</v>
       </c>
       <c r="I100">
-        <v>31</v>
-      </c>
-      <c r="J100" t="s">
-        <v>5</v>
-      </c>
-      <c r="K100">
+        <v>52</v>
+      </c>
+      <c r="J100">
         <v>30</v>
+      </c>
+      <c r="K100" t="s">
+        <v>5</v>
       </c>
       <c r="L100" t="s">
         <v>5</v>
@@ -4843,7 +4854,7 @@
         <v>5</v>
       </c>
       <c r="I101">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="J101" t="s">
         <v>5</v>
@@ -4859,38 +4870,152 @@
       <c r="A102" t="s">
         <v>101</v>
       </c>
-      <c r="B102" t="s">
-        <v>5</v>
+      <c r="B102">
+        <v>25</v>
       </c>
       <c r="C102" t="s">
         <v>5</v>
       </c>
-      <c r="D102" t="s">
-        <v>5</v>
+      <c r="D102">
+        <v>26</v>
       </c>
       <c r="E102" t="s">
         <v>5</v>
       </c>
-      <c r="F102" t="s">
-        <v>5</v>
+      <c r="F102">
+        <v>24</v>
       </c>
       <c r="G102" t="s">
         <v>5</v>
       </c>
-      <c r="H102" t="s">
-        <v>5</v>
+      <c r="H102">
+        <v>31</v>
       </c>
       <c r="I102" t="s">
         <v>5</v>
       </c>
       <c r="J102">
+        <v>30</v>
+      </c>
+      <c r="K102" t="s">
+        <v>5</v>
+      </c>
+      <c r="L102" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>5</v>
+      </c>
+      <c r="C103" t="s">
+        <v>5</v>
+      </c>
+      <c r="D103" t="s">
+        <v>5</v>
+      </c>
+      <c r="E103" t="s">
+        <v>5</v>
+      </c>
+      <c r="F103" t="s">
+        <v>5</v>
+      </c>
+      <c r="G103" t="s">
+        <v>5</v>
+      </c>
+      <c r="H103" t="s">
+        <v>5</v>
+      </c>
+      <c r="I103" t="s">
+        <v>5</v>
+      </c>
+      <c r="J103" t="s">
+        <v>5</v>
+      </c>
+      <c r="K103" t="s">
+        <v>5</v>
+      </c>
+      <c r="L103">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
+        <v>5</v>
+      </c>
+      <c r="C104" t="s">
+        <v>5</v>
+      </c>
+      <c r="D104" t="s">
+        <v>5</v>
+      </c>
+      <c r="E104" t="s">
+        <v>5</v>
+      </c>
+      <c r="F104" t="s">
+        <v>5</v>
+      </c>
+      <c r="G104" t="s">
+        <v>5</v>
+      </c>
+      <c r="H104">
+        <v>66</v>
+      </c>
+      <c r="I104" t="s">
+        <v>5</v>
+      </c>
+      <c r="J104" t="s">
+        <v>5</v>
+      </c>
+      <c r="K104" t="s">
+        <v>5</v>
+      </c>
+      <c r="L104" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
+        <v>5</v>
+      </c>
+      <c r="C105" t="s">
+        <v>5</v>
+      </c>
+      <c r="D105" t="s">
+        <v>5</v>
+      </c>
+      <c r="E105" t="s">
+        <v>5</v>
+      </c>
+      <c r="F105" t="s">
+        <v>5</v>
+      </c>
+      <c r="G105" t="s">
+        <v>5</v>
+      </c>
+      <c r="H105" t="s">
+        <v>5</v>
+      </c>
+      <c r="I105">
         <v>27</v>
       </c>
-      <c r="K102" t="s">
-        <v>5</v>
-      </c>
-      <c r="L102">
+      <c r="J105" t="s">
+        <v>5</v>
+      </c>
+      <c r="K105">
         <v>32</v>
+      </c>
+      <c r="L105">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>